<commit_message>
add a minor bug report
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UBCThings\Classes\CPSC 427\Team16\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F169E7AC-91FA-4A66-8BBB-8DF0320B931F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF2C1F5-986A-4B38-A137-42AE70FC2F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5850" yWindow="2850" windowWidth="20070" windowHeight="12285" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
   </bookViews>
   <sheets>
     <sheet name="bugs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>#</t>
   </si>
@@ -123,16 +123,31 @@
     <t>Jiayi</t>
   </si>
   <si>
-    <t>The animated player sprite is not updating consistently and may skip frame while walking</t>
-  </si>
-  <si>
-    <t>The sprite animates consistently in all directions</t>
-  </si>
-  <si>
-    <t>change player direction</t>
-  </si>
-  <si>
-    <t>The player sprite may stop updating upon change of direction</t>
+    <t>Ray</t>
+  </si>
+  <si>
+    <t>Change player direction in the game scene and the bug will appear.</t>
+  </si>
+  <si>
+    <t>Press two of the WASD keys in the main menu. Release one of them to enter the game scene while holding the other one. Release the other one in the game scene. The bug will then appear.</t>
+  </si>
+  <si>
+    <t>If two of the WASD keys are pressed in the main menu, the player may lose control in the game scene.</t>
+  </si>
+  <si>
+    <t>The animated player sprite is not updating consistently and may skip frame while walking.</t>
+  </si>
+  <si>
+    <t>The player sprite may stop updating upon change of direction.</t>
+  </si>
+  <si>
+    <t>The player should move according to the state of the WASD key.</t>
+  </si>
+  <si>
+    <t>The player keeps moving towards one direction.</t>
+  </si>
+  <si>
+    <t>The sprite should animate consistently in all directions.</t>
   </si>
 </sst>
 </file>
@@ -551,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699B0CA0-DDFC-4447-897A-42A4E259D7BB}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +579,7 @@
     <col min="7" max="7" width="51.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="47.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
@@ -624,15 +639,47 @@
         <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7">
+        <v>45578</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor wall collision bug fix
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UBCThings\Classes\CPSC 427\Team16\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF2C1F5-986A-4B38-A137-42AE70FC2F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07697F5D-80C2-42EA-92B2-3B22104706B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
   </bookViews>
@@ -630,7 +630,7 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Adds in a new bug
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UBCThings\Classes\CPSC 427\Team16\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07697F5D-80C2-42EA-92B2-3B22104706B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402417E1-0672-4781-98D2-5BF4D8A4585B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>#</t>
   </si>
@@ -148,6 +148,21 @@
   </si>
   <si>
     <t>The sprite should animate consistently in all directions.</t>
+  </si>
+  <si>
+    <t>resolved</t>
+  </si>
+  <si>
+    <t>The player should be blocked by the wall</t>
+  </si>
+  <si>
+    <t>The player keeps moving</t>
+  </si>
+  <si>
+    <t>If the player moves towards the bottom left corner of the map, they will pass through the wall</t>
+  </si>
+  <si>
+    <t>The player can squeeze themselves into a specific corner and pass through the wall</t>
   </si>
 </sst>
 </file>
@@ -566,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699B0CA0-DDFC-4447-897A-42A4E259D7BB}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +677,7 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
@@ -681,6 +696,38 @@
       </c>
       <c r="J5" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7">
+        <v>45578</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix and test plan
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UBCThings\Classes\CPSC 427\Team16\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0251DF6-0184-4FE1-95F8-E079D9CEB1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E4190D-A592-4F32-A41E-68A48FE9C795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="465" windowWidth="23700" windowHeight="12285" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
   </bookViews>
   <sheets>
     <sheet name="bugs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
   <si>
     <t>#</t>
   </si>
@@ -228,6 +228,18 @@
   </si>
   <si>
     <t>won't fix (can't reproduce)</t>
+  </si>
+  <si>
+    <t>Release WASD key while the game is frozen will cause the player to lose control and move indefinitely in one direciton.</t>
+  </si>
+  <si>
+    <t>The character should stop moving after the key is released</t>
+  </si>
+  <si>
+    <t>The chracter moves into one direction indefinitely</t>
+  </si>
+  <si>
+    <t>Press one of the WASD keys, drag the window to freeze it and then release the kay. After the game restores, the player will move into one direction indefinitely.</t>
   </si>
 </sst>
 </file>
@@ -662,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699B0CA0-DDFC-4447-897A-42A4E259D7BB}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,7 +775,7 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
         <v>28</v>
@@ -939,6 +951,38 @@
       </c>
       <c r="J10" s="1" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7">
+        <v>45613</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update test plan and bug report
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UBCThings\Classes\CPSC 427\Team16\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE5E9B0-77CE-40D4-B8D1-2BC775FB260B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908A1923-CE61-4580-8A4A-2D6CB5878ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
+    <workbookView xWindow="0" yWindow="3915" windowWidth="23700" windowHeight="12285" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
   </bookViews>
   <sheets>
     <sheet name="bugs" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>Yuntian</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>Jiayi</t>
   </si>
   <si>
@@ -252,6 +249,9 @@
   </si>
   <si>
     <t>Move the character around the enemy and there is a chance that you may find an angle such that the enemy thinks that she is overlapped with the player yet due to precise collision, no damage is dealt.</t>
+  </si>
+  <si>
+    <t>won't fix (this is Windows behaviour)</t>
   </si>
 </sst>
 </file>
@@ -688,15 +688,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699B0CA0-DDFC-4447-897A-42A4E259D7BB}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="51.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" style="1" customWidth="1"/>
@@ -755,22 +755,22 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="J4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -787,22 +787,22 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="J5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -819,22 +819,22 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -845,28 +845,28 @@
         <v>45598</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="J7" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -883,22 +883,22 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="J8" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -915,22 +915,22 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -941,28 +941,28 @@
         <v>45599</v>
       </c>
       <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
         <v>56</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="I10" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="J10" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -979,22 +979,22 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -1011,22 +1011,22 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
         <v>25</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more bug fix for tunnelling
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UBCThings\Classes\CPSC 427\Team16\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908A1923-CE61-4580-8A4A-2D6CB5878ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A8B00E-FFA0-4AB7-A1EF-9EF91E0B2FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3915" windowWidth="23700" windowHeight="12285" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
   </bookViews>
   <sheets>
     <sheet name="bugs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="84">
   <si>
     <t>#</t>
   </si>
@@ -197,10 +197,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>P2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>A consistant FPS rate regardless of devices</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -251,7 +247,43 @@
     <t>Move the character around the enemy and there is a chance that you may find an angle such that the enemy thinks that she is overlapped with the player yet due to precise collision, no damage is dealt.</t>
   </si>
   <si>
-    <t>won't fix (this is Windows behaviour)</t>
+    <t>Significant frame rate drop when entering large map</t>
+  </si>
+  <si>
+    <t>The frame rate should remain consistent across the gameplay</t>
+  </si>
+  <si>
+    <t>The frame rate will drop significantly if the player enters a large map</t>
+  </si>
+  <si>
+    <t>Enter the second map and the frame rate will drop significantly</t>
+  </si>
+  <si>
+    <t>Game crashes when the battery level reaches zero</t>
+  </si>
+  <si>
+    <t>Spider enemies will spawn around the player when battery level reaches zero</t>
+  </si>
+  <si>
+    <t>The game crashes</t>
+  </si>
+  <si>
+    <t>Wait until the battery level reaches zero</t>
+  </si>
+  <si>
+    <t>won't fix (This is Windows behaviour and there is no clean fix. This bug is uncommon to trigger unless intended. It is also easy to recover from this bug: just tap the corresponding key)</t>
+  </si>
+  <si>
+    <t>Player gets into the wall when dashing under low frame rate</t>
+  </si>
+  <si>
+    <t>Player's movement should be blocked by the wall</t>
+  </si>
+  <si>
+    <t>Player gets into the wall</t>
+  </si>
+  <si>
+    <t>Press space to dash towards the wall when frame rate is very low (&lt;20)</t>
   </si>
 </sst>
 </file>
@@ -686,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699B0CA0-DDFC-4447-897A-42A4E259D7BB}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,7 +731,7 @@
     <col min="5" max="5" width="35.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="51.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="47.85546875" style="1" customWidth="1"/>
   </cols>
@@ -769,7 +801,7 @@
       <c r="I4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="10" t="s">
         <v>28</v>
       </c>
     </row>
@@ -801,7 +833,7 @@
       <c r="I5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="10" t="s">
         <v>29</v>
       </c>
     </row>
@@ -833,11 +865,11 @@
       <c r="I6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>4</v>
       </c>
@@ -865,7 +897,7 @@
       <c r="I7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="10" t="s">
         <v>44</v>
       </c>
     </row>
@@ -883,7 +915,7 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F8" t="s">
         <v>46</v>
@@ -897,7 +929,7 @@
       <c r="I8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="10" t="s">
         <v>50</v>
       </c>
     </row>
@@ -923,13 +955,13 @@
       <c r="G9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="10" t="s">
         <v>54</v>
       </c>
     </row>
@@ -944,28 +976,28 @@
         <v>55</v>
       </c>
       <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="I10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="J10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>8</v>
       </c>
@@ -976,28 +1008,28 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>72</v>
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F11" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>9</v>
       </c>
@@ -1017,16 +1049,112 @@
         <v>25</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="J12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7">
+        <v>45628</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>71</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>11</v>
+      </c>
+      <c r="B14" s="7">
+        <v>45628</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>12</v>
+      </c>
+      <c r="B15" s="7">
+        <v>45628</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>